<commit_message>
grado 8, guion 05 - primera escaleta Flor
ajustes a escaleta según manuscrito revisado, por definir títulos de
recursos nuevos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion05/Escaleta_CS_08_05_CO - modelo nuevo.xlsx
+++ b/fuentes/contenidos/grado08/guion05/Escaleta_CS_08_05_CO - modelo nuevo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="149">
   <si>
     <t>Asignatura</t>
   </si>
@@ -393,6 +393,81 @@
   </si>
   <si>
     <t>La Revolución Industrial y el primer capitalismo</t>
+  </si>
+  <si>
+    <t>1 Los orígenes de la Revolución Industrial</t>
+  </si>
+  <si>
+    <t>1.1 La revolución agraria</t>
+  </si>
+  <si>
+    <t>1.2 La revolución demográfica</t>
+  </si>
+  <si>
+    <t>1.3 Consolidación</t>
+  </si>
+  <si>
+    <t>2 El nuevo modelo económico: el capitalismo</t>
+  </si>
+  <si>
+    <t>2.1 El capitalismo industrial</t>
+  </si>
+  <si>
+    <t>2.2 Consolidación</t>
+  </si>
+  <si>
+    <t>3 La primera Revolución Industrial (1750-1869)</t>
+  </si>
+  <si>
+    <t>3.1 El sistema fabril</t>
+  </si>
+  <si>
+    <t>3.2 La revolución de los transportes</t>
+  </si>
+  <si>
+    <t>3.3 Consolidación</t>
+  </si>
+  <si>
+    <t>4. La segunda Revolución Industrial (1869-1910)</t>
+  </si>
+  <si>
+    <t>4.1 Las nuevas fuentes de energía</t>
+  </si>
+  <si>
+    <t>4.2 Las nuevas industrias</t>
+  </si>
+  <si>
+    <t>4.3 Los nuevos sistemas de producción</t>
+  </si>
+  <si>
+    <t>4.4 Consolidación</t>
+  </si>
+  <si>
+    <t>5 Las consecuencias de la Revolución Industrial</t>
+  </si>
+  <si>
+    <t>5.1 Consolidación</t>
+  </si>
+  <si>
+    <t>6 Competencias</t>
+  </si>
+  <si>
+    <t>Competencias</t>
+  </si>
+  <si>
+    <t>Proyecto</t>
+  </si>
+  <si>
+    <t>Fin de tema</t>
+  </si>
+  <si>
+    <t>Evaluación</t>
+  </si>
+  <si>
+    <t>Webs de referencia</t>
+  </si>
+  <si>
+    <t>Banco de contenidos</t>
   </si>
 </sst>
 </file>
@@ -625,7 +700,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -662,13 +737,51 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -704,47 +817,12 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3017,8 +3095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3028,10 +3106,10 @@
     <col min="3" max="3" width="18.42578125" style="10" customWidth="1"/>
     <col min="4" max="4" width="34.140625" style="8" customWidth="1"/>
     <col min="5" max="5" width="32.85546875" style="24" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" style="17" customWidth="1"/>
-    <col min="7" max="7" width="36.5703125" style="15" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="15" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" style="15" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" style="17" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="33.85546875" style="15" customWidth="1"/>
+    <col min="8" max="8" width="9" style="59" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="15" customWidth="1"/>
     <col min="10" max="10" width="30.28515625" style="15" customWidth="1"/>
     <col min="11" max="11" width="18.85546875" style="23" customWidth="1"/>
     <col min="12" max="12" width="21.5703125" style="23" customWidth="1"/>
@@ -3047,133 +3125,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="K1" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="L1" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="M1" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="36"/>
-      <c r="O1" s="30" t="s">
+      <c r="N1" s="52"/>
+      <c r="O1" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="42" t="s">
+      <c r="P1" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="Q1" s="43" t="s">
+      <c r="Q1" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="45" t="s">
+      <c r="R1" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="S1" s="43" t="s">
+      <c r="S1" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="44" t="s">
+      <c r="T1" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="U1" s="43" t="s">
+      <c r="U1" s="42" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
       <c r="M2" s="21" t="s">
         <v>92</v>
       </c>
       <c r="N2" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="45"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="43"/>
-    </row>
-    <row r="3" spans="1:21" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="42"/>
+    </row>
+    <row r="3" spans="1:21" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="56"/>
-      <c r="S3" s="55"/>
-      <c r="T3" s="57"/>
-      <c r="U3" s="55"/>
+      <c r="D3" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="31"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33">
+        <v>1</v>
+      </c>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="36"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="36"/>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="11"/>
       <c r="C4" s="9"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="F4" s="16"/>
       <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="H4" s="58">
+        <v>2</v>
+      </c>
       <c r="I4" s="13"/>
       <c r="J4" s="14"/>
       <c r="K4" s="22"/>
@@ -3192,11 +3277,14 @@
       <c r="A5" s="18"/>
       <c r="B5" s="11"/>
       <c r="C5" s="9"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="F5" s="16"/>
       <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+      <c r="H5" s="58">
+        <v>3</v>
+      </c>
       <c r="I5" s="13"/>
       <c r="J5" s="14"/>
       <c r="K5" s="22"/>
@@ -3215,11 +3303,14 @@
       <c r="A6" s="18"/>
       <c r="B6" s="11"/>
       <c r="C6" s="20"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="F6" s="16"/>
       <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="H6" s="58">
+        <v>4</v>
+      </c>
       <c r="I6" s="13"/>
       <c r="J6" s="14"/>
       <c r="K6" s="22"/>
@@ -3238,11 +3329,15 @@
       <c r="A7" s="18"/>
       <c r="B7" s="11"/>
       <c r="C7" s="9"/>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>128</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="16"/>
       <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="H7" s="58">
+        <v>5</v>
+      </c>
       <c r="I7" s="13"/>
       <c r="J7" s="14"/>
       <c r="K7" s="22"/>
@@ -3261,11 +3356,14 @@
       <c r="A8" s="18"/>
       <c r="B8" s="11"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="F8" s="16"/>
       <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
+      <c r="H8" s="58">
+        <v>6</v>
+      </c>
       <c r="I8" s="13"/>
       <c r="J8" s="14"/>
       <c r="K8" s="22"/>
@@ -3284,11 +3382,14 @@
       <c r="A9" s="18"/>
       <c r="B9" s="11"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="F9" s="16"/>
       <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
+      <c r="H9" s="58">
+        <v>7</v>
+      </c>
       <c r="I9" s="13"/>
       <c r="J9" s="14"/>
       <c r="K9" s="22"/>
@@ -3307,11 +3408,14 @@
       <c r="A10" s="18"/>
       <c r="B10" s="11"/>
       <c r="C10" s="9"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
+      <c r="D10" s="2" t="s">
+        <v>131</v>
+      </c>
       <c r="F10" s="16"/>
       <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="H10" s="58">
+        <v>8</v>
+      </c>
       <c r="I10" s="13"/>
       <c r="J10" s="14"/>
       <c r="K10" s="22"/>
@@ -3330,11 +3434,14 @@
       <c r="A11" s="18"/>
       <c r="B11" s="11"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="F11" s="16"/>
       <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+      <c r="H11" s="58">
+        <v>9</v>
+      </c>
       <c r="I11" s="13"/>
       <c r="J11" s="14"/>
       <c r="K11" s="22"/>
@@ -3353,11 +3460,14 @@
       <c r="A12" s="18"/>
       <c r="B12" s="11"/>
       <c r="C12" s="9"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="F12" s="16"/>
       <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="H12" s="58">
+        <v>10</v>
+      </c>
       <c r="I12" s="13"/>
       <c r="J12" s="14"/>
       <c r="K12" s="22"/>
@@ -3376,11 +3486,14 @@
       <c r="A13" s="18"/>
       <c r="B13" s="11"/>
       <c r="C13" s="9"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>134</v>
+      </c>
       <c r="F13" s="16"/>
       <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="H13" s="58">
+        <v>11</v>
+      </c>
       <c r="I13" s="13"/>
       <c r="J13" s="14"/>
       <c r="K13" s="22"/>
@@ -3399,11 +3512,15 @@
       <c r="A14" s="18"/>
       <c r="B14" s="11"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>135</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="16"/>
       <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
+      <c r="H14" s="58">
+        <v>12</v>
+      </c>
       <c r="I14" s="13"/>
       <c r="J14" s="14"/>
       <c r="K14" s="22"/>
@@ -3422,11 +3539,14 @@
       <c r="A15" s="18"/>
       <c r="B15" s="11"/>
       <c r="C15" s="9"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="F15" s="16"/>
       <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
+      <c r="H15" s="58">
+        <v>13</v>
+      </c>
       <c r="I15" s="13"/>
       <c r="J15" s="14"/>
       <c r="K15" s="22"/>
@@ -3445,11 +3565,14 @@
       <c r="A16" s="18"/>
       <c r="B16" s="11"/>
       <c r="C16" s="9"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="F16" s="16"/>
       <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
+      <c r="H16" s="58">
+        <v>14</v>
+      </c>
       <c r="I16" s="13"/>
       <c r="J16" s="14"/>
       <c r="K16" s="22"/>
@@ -3468,11 +3591,14 @@
       <c r="A17" s="18"/>
       <c r="B17" s="11"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="F17" s="16"/>
       <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
+      <c r="H17" s="58">
+        <v>15</v>
+      </c>
       <c r="I17" s="13"/>
       <c r="J17" s="14"/>
       <c r="K17" s="22"/>
@@ -3491,11 +3617,14 @@
       <c r="A18" s="18"/>
       <c r="B18" s="11"/>
       <c r="C18" s="9"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="F18" s="16"/>
       <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="H18" s="58">
+        <v>16</v>
+      </c>
       <c r="I18" s="13"/>
       <c r="J18" s="14"/>
       <c r="K18" s="22"/>
@@ -3514,11 +3643,15 @@
       <c r="A19" s="18"/>
       <c r="B19" s="11"/>
       <c r="C19" s="9"/>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>140</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="16"/>
       <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
+      <c r="H19" s="58">
+        <v>17</v>
+      </c>
       <c r="I19" s="13"/>
       <c r="J19" s="14"/>
       <c r="K19" s="22"/>
@@ -3537,11 +3670,14 @@
       <c r="A20" s="18"/>
       <c r="B20" s="11"/>
       <c r="C20" s="9"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="F20" s="16"/>
       <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
+      <c r="H20" s="58">
+        <v>18</v>
+      </c>
       <c r="I20" s="13"/>
       <c r="J20" s="14"/>
       <c r="K20" s="22"/>
@@ -3560,11 +3696,13 @@
       <c r="A21" s="18"/>
       <c r="B21" s="11"/>
       <c r="C21" s="9"/>
-      <c r="D21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="E21" s="1"/>
       <c r="F21" s="16"/>
       <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
+      <c r="H21" s="58"/>
       <c r="I21" s="13"/>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -3583,11 +3721,14 @@
       <c r="A22" s="18"/>
       <c r="B22" s="11"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="F22" s="16"/>
       <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
+      <c r="H22" s="58">
+        <v>19</v>
+      </c>
       <c r="I22" s="13"/>
       <c r="J22" s="14"/>
       <c r="K22" s="22"/>
@@ -3606,11 +3747,14 @@
       <c r="A23" s="18"/>
       <c r="B23" s="11"/>
       <c r="C23" s="9"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="F23" s="16"/>
       <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
+      <c r="H23" s="58">
+        <v>20</v>
+      </c>
       <c r="I23" s="13"/>
       <c r="J23" s="14"/>
       <c r="K23" s="22"/>
@@ -3629,11 +3773,12 @@
       <c r="A24" s="18"/>
       <c r="B24" s="11"/>
       <c r="C24" s="9"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="1"/>
+      <c r="D24" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="F24" s="16"/>
       <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
+      <c r="H24" s="58"/>
       <c r="I24" s="13"/>
       <c r="J24" s="14"/>
       <c r="K24" s="22"/>
@@ -3652,11 +3797,14 @@
       <c r="A25" s="18"/>
       <c r="B25" s="11"/>
       <c r="C25" s="9"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="F25" s="16"/>
       <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
+      <c r="H25" s="58">
+        <v>21</v>
+      </c>
       <c r="I25" s="13"/>
       <c r="J25" s="14"/>
       <c r="K25" s="22"/>
@@ -3675,11 +3823,14 @@
       <c r="A26" s="18"/>
       <c r="B26" s="11"/>
       <c r="C26" s="9"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>146</v>
+      </c>
       <c r="F26" s="16"/>
       <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
+      <c r="H26" s="58">
+        <v>22</v>
+      </c>
       <c r="I26" s="13"/>
       <c r="J26" s="14"/>
       <c r="K26" s="22"/>
@@ -3698,11 +3849,12 @@
       <c r="A27" s="18"/>
       <c r="B27" s="11"/>
       <c r="C27" s="9"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>147</v>
+      </c>
       <c r="F27" s="16"/>
       <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
+      <c r="H27" s="58"/>
       <c r="I27" s="13"/>
       <c r="J27" s="14"/>
       <c r="K27" s="22"/>
@@ -3721,11 +3873,14 @@
       <c r="A28" s="18"/>
       <c r="B28" s="11"/>
       <c r="C28" s="9"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>148</v>
+      </c>
       <c r="F28" s="16"/>
       <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
+      <c r="H28" s="58">
+        <v>23</v>
+      </c>
       <c r="I28" s="13"/>
       <c r="J28" s="14"/>
       <c r="K28" s="22"/>
@@ -3748,7 +3903,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="16"/>
       <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
+      <c r="H29" s="58"/>
       <c r="I29" s="13"/>
       <c r="J29" s="14"/>
       <c r="K29" s="22"/>
@@ -3771,7 +3926,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="16"/>
       <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
+      <c r="H30" s="58"/>
       <c r="I30" s="13"/>
       <c r="J30" s="14"/>
       <c r="K30" s="22"/>
@@ -3794,7 +3949,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="16"/>
       <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
+      <c r="H31" s="58"/>
       <c r="I31" s="13"/>
       <c r="J31" s="14"/>
       <c r="K31" s="22"/>
@@ -3817,7 +3972,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="16"/>
       <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
+      <c r="H32" s="58"/>
       <c r="I32" s="13"/>
       <c r="J32" s="14"/>
       <c r="K32" s="22"/>
@@ -3840,7 +3995,7 @@
       <c r="E33" s="1"/>
       <c r="F33" s="16"/>
       <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
+      <c r="H33" s="58"/>
       <c r="I33" s="13"/>
       <c r="J33" s="14"/>
       <c r="K33" s="22"/>
@@ -3863,7 +4018,7 @@
       <c r="E34" s="1"/>
       <c r="F34" s="16"/>
       <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
+      <c r="H34" s="58"/>
       <c r="I34" s="13"/>
       <c r="J34" s="14"/>
       <c r="K34" s="22"/>
@@ -3886,7 +4041,7 @@
       <c r="E35" s="1"/>
       <c r="F35" s="16"/>
       <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
+      <c r="H35" s="58"/>
       <c r="I35" s="13"/>
       <c r="J35" s="14"/>
       <c r="K35" s="22"/>
@@ -3909,7 +4064,7 @@
       <c r="E36" s="1"/>
       <c r="F36" s="16"/>
       <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
+      <c r="H36" s="58"/>
       <c r="I36" s="13"/>
       <c r="J36" s="14"/>
       <c r="K36" s="22"/>
@@ -3932,7 +4087,7 @@
       <c r="E37" s="1"/>
       <c r="F37" s="16"/>
       <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
+      <c r="H37" s="58"/>
       <c r="I37" s="13"/>
       <c r="J37" s="14"/>
       <c r="K37" s="22"/>
@@ -3955,7 +4110,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="16"/>
       <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
+      <c r="H38" s="58"/>
       <c r="I38" s="13"/>
       <c r="J38" s="14"/>
       <c r="K38" s="22"/>
@@ -3978,7 +4133,7 @@
       <c r="E39" s="1"/>
       <c r="F39" s="16"/>
       <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
+      <c r="H39" s="58"/>
       <c r="I39" s="13"/>
       <c r="J39" s="14"/>
       <c r="K39" s="22"/>
@@ -4001,7 +4156,7 @@
       <c r="E40" s="1"/>
       <c r="F40" s="16"/>
       <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
+      <c r="H40" s="58"/>
       <c r="I40" s="13"/>
       <c r="J40" s="14"/>
       <c r="K40" s="22"/>
@@ -4024,7 +4179,7 @@
       <c r="E41" s="1"/>
       <c r="F41" s="16"/>
       <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
+      <c r="H41" s="58"/>
       <c r="I41" s="13"/>
       <c r="J41" s="14"/>
       <c r="K41" s="22"/>
@@ -4226,12 +4381,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="B1:B2"/>
@@ -4246,6 +4395,12 @@
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="I1:I2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>